<commit_message>
Buffer implemented. advance matrix pending,
</commit_message>
<xml_diff>
--- a/DFA.xlsx
+++ b/DFA.xlsx
@@ -202,10 +202,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>N_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -272,16 +269,19 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>N_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell/>
+          <table:table-cell table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N_FINAL</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="28"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>YES</text:p>
+          </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>NO</text:p>
           </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N_FINAL</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="30"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
@@ -294,7 +294,11 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>I1</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="25"/>
+          <table:table-cell table:number-columns-repeated="22"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_CHECK</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
@@ -314,7 +318,13 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>I_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="30"/>
+          <table:table-cell table:number-columns-repeated="28"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>YES</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NO</text:p>
+          </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
@@ -328,10 +338,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>O_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
@@ -345,10 +352,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>O_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
@@ -362,10 +366,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>O_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
@@ -382,10 +383,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>O_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
@@ -402,10 +400,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>O_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
@@ -417,12 +412,9 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="11"/>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>O_FINAL</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+            <text:p>ERROR</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
@@ -474,13 +466,37 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>P_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="30"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>O_FINAL</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="30"/>
+          <table:table-cell table:number-columns-repeated="28"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>YES</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NO</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>O_FINAL</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="28"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>YES</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NO</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_CHECK</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="28"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>MAYBE</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NO</text:p>
+          </table:table-cell>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -493,11 +509,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-03-08T20:39:15.192185133</meta:creation-date>
-    <dc:date>2025-03-10T20:39:37.502060986</dc:date>
-    <meta:editing-duration>PT31M20S</meta:editing-duration>
-    <meta:editing-cycles>5</meta:editing-cycles>
+    <dc:date>2025-03-12T02:15:21.546221869</dc:date>
+    <meta:editing-duration>PT1H5M3S</meta:editing-duration>
+    <meta:editing-cycles>6</meta:editing-cycles>
     <meta:generator>LibreOffice/24.2.7.2$Linux_X86_64 LibreOffice_project/420$Build-2</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="130" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="134" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -509,21 +525,21 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">72233</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">10386</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">10837</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">7</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">13</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">30</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">20</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">2</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">2</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">1</config:config-item>
               <config:config-item config:name="VerticalSplitPosition" config:type="int">1</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">3</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionRight" config:type="int">1</config:config-item>
+              <config:config-item config:name="PositionRight" config:type="int">19</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">1</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
@@ -598,7 +614,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">wAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMArAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsJzAsMApjb2xvcmRlcHRoPTI0CmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6QTQARHVwbGV4Ok5vbmUAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmYMAFBSSU5URVJfTkFNRQ8AR2VuZXJpYyBQcmludGVyCwBEUklWRVJfTkFNRQcAU0dFTlBSVA==</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">wAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMArAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsJzAsMApjb2xvcmRlcHRoPTI0CmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmYMAFBSSU5URVJfTkFNRQ8AR2VuZXJpYyBQcmludGVyCwBEUklWRVJfTkFNRQcAU0dFTlBSVA==</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
@@ -650,25 +666,12 @@
     <number:number-style style:name="N0">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
-    <number:currency-style style:name="N129P0" style:volatile="true">
+    <number:currency-style style:name="N130P0" style:volatile="true">
       <number:currency-symbol/>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N129">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N129P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N130P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
+      <number:text> _)</number:text>
     </number:currency-style>
     <number:currency-style style:name="N130">
-      <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
@@ -677,61 +680,74 @@
     </number:currency-style>
     <number:currency-style style:name="N131P0" style:volatile="true">
       <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> _)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N131">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N131P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N133P0" style:volatile="true">
+      <number:currency-symbol/>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N131">
+      <number:text> _)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N133">
       <number:text>(</number:text>
       <number:currency-symbol/>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N131P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N132P0" style:volatile="true">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N133P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N134P0" style:volatile="true">
       <number:currency-symbol/>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N132">
+      <number:text> _)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N134">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N132P0"/>
-    </number:currency-style>
-    <number:date-style style:name="N133">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N134P0"/>
+    </number:currency-style>
+    <number:date-style style:name="N135">
       <number:month/>
       <number:text>/</number:text>
       <number:day/>
       <number:text>/</number:text>
       <number:year number:style="long"/>
     </number:date-style>
-    <number:date-style style:name="N134">
+    <number:date-style style:name="N136">
       <number:day/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:date-style style:name="N135">
+    <number:date-style style:name="N137">
       <number:day/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
     </number:date-style>
-    <number:date-style style:name="N136">
+    <number:date-style style:name="N138">
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:time-style style:name="N137">
+    <number:time-style style:name="N139">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text> </number:text>
       <number:am-pm/>
     </number:time-style>
-    <number:time-style style:name="N138">
+    <number:time-style style:name="N140">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
@@ -740,19 +756,19 @@
       <number:text> </number:text>
       <number:am-pm/>
     </number:time-style>
-    <number:time-style style:name="N139">
+    <number:time-style style:name="N141">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N140">
+    <number:time-style style:name="N142">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:date-style style:name="N141">
+    <number:date-style style:name="N143">
       <number:month/>
       <number:text>/</number:text>
       <number:day/>
@@ -763,62 +779,62 @@
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
     </number:date-style>
-    <number:number-style style:name="N142P0" style:volatile="true">
+    <number:number-style style:name="N145P0" style:volatile="true">
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text loext:blank-width-char=")"> </number:text>
     </number:number-style>
-    <number:number-style style:name="N142">
+    <number:number-style style:name="N145">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N142P0"/>
-    </number:number-style>
-    <number:number-style style:name="N143P0" style:volatile="true">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N145P0"/>
+    </number:number-style>
+    <number:number-style style:name="N147P0" style:volatile="true">
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text loext:blank-width-char=")"> </number:text>
     </number:number-style>
-    <number:number-style style:name="N143">
+    <number:number-style style:name="N147">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N143P0"/>
-    </number:number-style>
-    <number:number-style style:name="N144P0" style:volatile="true">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N147P0"/>
+    </number:number-style>
+    <number:number-style style:name="N151P0" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text loext:blank-width-char=")"> </number:text>
     </number:number-style>
-    <number:number-style style:name="N144P1" style:volatile="true">
+    <number:number-style style:name="N151P1" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
-    <number:number-style style:name="N144P2" style:volatile="true">
+    <number:number-style style:name="N151P2" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:fill-character> </number:fill-character>
-      <number:text loext:blank-width-char=")1">- </number:text>
-    </number:number-style>
-    <number:text-style style:name="N144">
+      <number:text>- _)</number:text>
+    </number:number-style>
+    <number:text-style style:name="N151">
       <number:text loext:blank-width-char="("> </number:text>
       <number:text-content/>
       <number:text loext:blank-width-char=")"> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N144P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N144P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N144P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N151P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N151P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N151P2"/>
     </number:text-style>
-    <number:currency-style style:name="N145P0" style:volatile="true">
+    <number:currency-style style:name="N155P0" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N145P1" style:volatile="true">
+      <number:text> _)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N155P1" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
@@ -826,56 +842,56 @@
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:currency-style>
-    <number:currency-style style:name="N145P2" style:volatile="true">
+    <number:currency-style style:name="N155P2" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
-      <number:text loext:blank-width-char=")1">- </number:text>
-    </number:currency-style>
-    <number:text-style style:name="N145">
+      <number:text>- _)</number:text>
+    </number:currency-style>
+    <number:text-style style:name="N155">
       <number:text loext:blank-width-char="("> </number:text>
       <number:text-content/>
       <number:text loext:blank-width-char=")"> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N145P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N145P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N145P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N155P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N155P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N155P2"/>
     </number:text-style>
-    <number:number-style style:name="N146P0" style:volatile="true">
+    <number:number-style style:name="N159P0" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text loext:blank-width-char=")"> </number:text>
     </number:number-style>
-    <number:number-style style:name="N146P1" style:volatile="true">
+    <number:number-style style:name="N159P1" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>(</number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
-    <number:number-style style:name="N146P2" style:volatile="true">
+    <number:number-style style:name="N159P2" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="2" loext:max-blank-integer-digits="2"/>
       <number:text loext:blank-width-char=")"> </number:text>
     </number:number-style>
-    <number:text-style style:name="N146">
+    <number:text-style style:name="N159">
       <number:text loext:blank-width-char="("> </number:text>
       <number:text-content/>
       <number:text loext:blank-width-char=")"> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N146P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N146P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N146P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N159P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N159P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N159P2"/>
     </number:text-style>
-    <number:currency-style style:name="N147P0" style:volatile="true">
+    <number:currency-style style:name="N163P0" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text loext:blank-width-char=")"> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N147P1" style:volatile="true">
+      <number:text> _)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N163P1" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
@@ -883,40 +899,40 @@
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:currency-style>
-    <number:currency-style style:name="N147P2" style:volatile="true">
+    <number:currency-style style:name="N163P2" style:volatile="true">
       <number:text loext:blank-width-char="("> </number:text>
       <number:currency-symbol/>
       <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="2" loext:max-blank-integer-digits="2"/>
-      <number:text loext:blank-width-char=")"> </number:text>
-    </number:currency-style>
-    <number:text-style style:name="N147">
+      <number:text> _)</number:text>
+    </number:currency-style>
+    <number:text-style style:name="N163">
       <number:text loext:blank-width-char="("> </number:text>
       <number:text-content/>
       <number:text loext:blank-width-char=")"> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N147P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N147P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N147P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N163P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N163P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N163P2"/>
     </number:text-style>
-    <number:time-style style:name="N148">
+    <number:time-style style:name="N164">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N149" number:truncate-on-overflow="false">
+    <number:time-style style:name="N165" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N150">
+    <number:time-style style:name="N166">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:number-style style:name="N151">
+    <number:number-style style:name="N167">
       <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
     </number:number-style>
     <style:style style:name="Default" style:family="table-cell"/>
@@ -1065,9 +1081,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2025-03-11">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2025-03-12">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="19:58:06.026909482">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="23:46:18.176732963">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
lexer complete. need to change suymbol table to a composite tree
</commit_message>
<xml_diff>
--- a/DFA.xlsx
+++ b/DFA.xlsx
@@ -131,9 +131,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>FINAL</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ADVANCE</text:p>
-          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -186,7 +184,10 @@
           <table:table-cell table:number-columns-repeated="4" office:value-type="string" calcext:value-type="string">
             <text:p>O_FINAL</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="4"/>
+          <table:table-cell table:number-columns-repeated="3"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NO</text:p>
+          </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
@@ -215,7 +216,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>ERROR</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NO</text:p>
+          </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
@@ -259,7 +263,10 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>ERROR</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NO</text:p>
+          </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
@@ -279,9 +286,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>YES</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
@@ -322,9 +327,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>YES</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
@@ -470,9 +473,7 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>YES</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -482,21 +483,82 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>YES</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>K_CHECK</text:p>
           </table:table-cell>
+          <table:table-cell table:number-columns-repeated="27"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ERROR</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>MAYBE</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_OUTPUT</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="13"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_OUTPUT_LT</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="13"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ERROR</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_INPUT</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="17"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_INPUT_SUB</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="9"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ERROR</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_OUTPUT_LT</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="17"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_FINAL</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="9"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ERROR</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_INPUT_SUB</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="14"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_FINAL</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="15"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>K_FINAL</text:p>
+          </table:table-cell>
           <table:table-cell table:number-columns-repeated="28"/>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>MAYBE</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NO</text:p>
-          </table:table-cell>
+            <text:p>YES</text:p>
+          </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -509,11 +571,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-03-08T20:39:15.192185133</meta:creation-date>
-    <dc:date>2025-03-12T02:15:21.546221869</dc:date>
-    <meta:editing-duration>PT1H5M3S</meta:editing-duration>
-    <meta:editing-cycles>6</meta:editing-cycles>
+    <dc:date>2025-03-16T21:20:05.392240636</dc:date>
+    <meta:editing-duration>PT2H54M49S</meta:editing-duration>
+    <meta:editing-cycles>8</meta:editing-cycles>
     <meta:generator>LibreOffice/24.2.7.2$Linux_X86_64 LibreOffice_project/420$Build-2</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="134" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="145" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -525,21 +587,21 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">72233</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">10837</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">13095</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">30</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">20</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">15</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">28</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">2</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">2</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">1</config:config-item>
               <config:config-item config:name="VerticalSplitPosition" config:type="int">1</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">3</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionRight" config:type="int">19</config:config-item>
+              <config:config-item config:name="PositionRight" config:type="int">7</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">1</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
@@ -1081,9 +1143,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2025-03-12">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2025-03-16">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="23:46:18.176732963">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="19:32:04.740637988">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>